<commit_message>
Update Bill of Materials - Hypnos V3.1.xlsx
</commit_message>
<xml_diff>
--- a/Hypnos 12V/Bill of Materials - Hypnos V3.1.xlsx
+++ b/Hypnos 12V/Bill of Materials - Hypnos V3.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao Nguyen\Documents\GitHub\OPEnS-Power\Hypnos 12V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403F7DD9-1889-4E21-845C-CDE68BE9D458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91762ED-3A05-466E-A5BA-EC7749AC972E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Mouser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="81">
   <si>
     <t>Digikey</t>
   </si>
@@ -196,9 +197,6 @@
     <t>100k resistor 1%</t>
   </si>
   <si>
-    <t>311-100KCRCT-ND</t>
-  </si>
-  <si>
     <t>100pF Capacitor</t>
   </si>
   <si>
@@ -278,6 +276,9 @@
   </si>
   <si>
     <t>SOT26-6</t>
+  </si>
+  <si>
+    <t>311-100KFRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -753,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -813,7 +814,7 @@
         <v>0.66</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>8</v>
@@ -824,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -840,7 +841,7 @@
         <v>0.41</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>27</v>
@@ -867,7 +868,7 @@
         <v>0.34</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>49</v>
@@ -889,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E6" s="5">
         <v>0.1</v>
@@ -899,9 +900,11 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="13"/>
+        <v>63</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -924,7 +927,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="13">
         <v>1206</v>
@@ -951,7 +954,7 @@
         <v>1.95</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="13"/>
     </row>
@@ -976,7 +979,7 @@
         <v>8.77</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" s="13"/>
     </row>
@@ -1004,7 +1007,7 @@
         <v>0.68</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>24</v>
@@ -1031,7 +1034,7 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="18"/>
     </row>
@@ -1055,7 +1058,7 @@
         <v>0.1</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" s="18">
         <v>1206</v>
@@ -1082,7 +1085,7 @@
         <v>0.38</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="18">
         <v>1206</v>
@@ -1109,7 +1112,7 @@
         <v>1.02</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="19" t="s">
         <v>27</v>
@@ -1120,13 +1123,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="15">
-        <v>1</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>58</v>
       </c>
       <c r="E16" s="15">
         <v>0.1</v>
@@ -1136,7 +1139,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>28</v>
@@ -1147,13 +1150,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" s="15">
-        <v>1</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="E17" s="15">
         <v>0.1</v>
@@ -1163,7 +1166,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>28</v>
@@ -1174,13 +1177,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" s="15">
-        <v>2</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="E18" s="15">
         <v>0.1</v>
@@ -1190,7 +1193,7 @@
         <v>0.2</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>27</v>
@@ -1201,13 +1204,13 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="E19">
         <v>0.44</v>
@@ -1217,7 +1220,7 @@
         <v>0.44</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K19" s="13"/>
     </row>
@@ -1270,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B778148E-242D-409E-9127-666EF26A5862}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="15">
         <v>0.15</v>
@@ -1332,7 +1335,7 @@
         <v>0.15</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -1362,7 +1365,7 @@
         <v>0.62</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -1376,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1392,7 +1395,7 @@
         <v>0.41</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -1425,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="15">
         <v>0.1</v>
@@ -1435,7 +1438,7 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -1465,7 +1468,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
@@ -1495,7 +1498,7 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -1526,7 +1529,7 @@
         <v>8.77</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -1567,7 +1570,7 @@
         <v>0.66</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -1600,7 +1603,7 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -1628,7 +1631,7 @@
         <v>0.18</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -1658,7 +1661,7 @@
         <v>0.36</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -1688,7 +1691,7 @@
         <v>0.86</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -1702,13 +1705,13 @@
         <v>30</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="15">
         <v>1</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="15">
         <v>0.1</v>
@@ -1718,7 +1721,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -1732,13 +1735,13 @@
         <v>30</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="15">
         <v>0.1</v>
@@ -1748,7 +1751,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -1762,13 +1765,13 @@
         <v>30</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15">
         <v>2</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="15">
         <v>0.1</v>
@@ -1778,7 +1781,7 @@
         <v>0.2</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -1792,13 +1795,13 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="E19">
         <v>0.44</v>
@@ -1808,10 +1811,10 @@
         <v>0.44</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
@@ -1862,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00EFBA5-BB63-4E95-AAB6-77207EAA5FF2}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,7 +1915,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>0.16</v>
@@ -1922,7 +1925,7 @@
         <v>0.32</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="24" t="s">
         <v>8</v>
@@ -1949,7 +1952,7 @@
         <v>0.66</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>8</v>
@@ -1960,13 +1963,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="5">
         <v>0.39</v>
@@ -1976,10 +1979,10 @@
         <v>0.39</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2006,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="15">
         <v>0.1</v>
@@ -2016,7 +2019,7 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -2036,7 +2039,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7">
         <v>0.1</v>
@@ -2046,7 +2049,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7" s="24">
         <v>1206</v>
@@ -2073,7 +2076,7 @@
         <v>1.95</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="24"/>
     </row>
@@ -2098,7 +2101,7 @@
         <v>9.0399999999999991</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" s="24"/>
     </row>
@@ -2128,7 +2131,7 @@
         <v>0.68</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="24" t="s">
         <v>24</v>
@@ -2155,7 +2158,7 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="24"/>
     </row>
@@ -2170,7 +2173,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="12">
         <v>0.15</v>
@@ -2180,7 +2183,7 @@
         <v>0.3</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K13" s="24">
         <v>1206</v>
@@ -2207,7 +2210,7 @@
         <v>0.52</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="24">
         <v>1206</v>
@@ -2234,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K15" s="25" t="s">
         <v>27</v>
@@ -2245,13 +2248,13 @@
         <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16">
         <v>0.1</v>
@@ -2261,7 +2264,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>28</v>
@@ -2272,13 +2275,13 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17">
         <v>0.23</v>
@@ -2288,7 +2291,7 @@
         <v>0.23</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>28</v>
@@ -2299,13 +2302,13 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18">
         <v>0.1</v>
@@ -2315,7 +2318,7 @@
         <v>0.2</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K18" s="25" t="s">
         <v>27</v>
@@ -2326,13 +2329,13 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19">
         <v>0.44</v>
@@ -2342,10 +2345,10 @@
         <v>0.44</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K19" s="25"/>
     </row>

</xml_diff>